<commit_message>
chore: change export data of ledger
</commit_message>
<xml_diff>
--- a/templates/transactions/ledger.xlsx
+++ b/templates/transactions/ledger.xlsx
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -49,9 +51,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -417,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,116 +432,62 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>TITLE</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>DATE</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>TITLE</t>
-        </is>
-      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>CURRENCY</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>DEBIT AMOUNT</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>CREDIT AMOUNT</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>NARRATION</t>
+          <t>TIME</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-10-06</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Clearance</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>MZN</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>money transfer to xyz</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2023-10-06</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Clearance</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>MZN</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>950</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>money transfer to xyz</t>
-        </is>
+          <t>Cash To Mustafa</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>45206</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>0.7096339854976852</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2023-10-06</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Clearance</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>MZN</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>999</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>money transfer to xyz</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>DATE</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>TITLE</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>CURRENCY</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>DEBIT AMOUNT</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>CREDIT AMOUNT</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>NARRATION</t>
         </is>
       </c>
     </row>
@@ -558,10 +508,10 @@
         </is>
       </c>
       <c r="D5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E5" t="n">
         <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -582,14 +532,14 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>MZN</t>
         </is>
       </c>
       <c r="D6" t="n">
+        <v>950</v>
+      </c>
+      <c r="E6" t="n">
         <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>4440</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -610,16 +560,100 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>MZN</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>55</v>
+        <v>999</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="inlineStr">
+        <is>
+          <t>money transfer to xyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-10-06</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Clearance</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>MZN</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>money transfer to xyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-10-06</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Clearance</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4440</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>money transfer to xyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2023-10-06</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Clearance</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>55</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="inlineStr">
         <is>
           <t>money transfer to xyz</t>
         </is>

</xml_diff>

<commit_message>
fix: change api method
</commit_message>
<xml_diff>
--- a/templates/transactions/ledger.xlsx
+++ b/templates/transactions/ledger.xlsx
@@ -453,10 +453,10 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45206</v>
+        <v>45217</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>0.7096339854976852</v>
+        <v>0.8542566528125</v>
       </c>
     </row>
     <row r="4">

</xml_diff>